<commit_message>
App Design file added to have an idea of how the app has to be like
</commit_message>
<xml_diff>
--- a/Objectives.xlsx
+++ b/Objectives.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Objectif</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Changer le JSON Settings, enlever le TestType etc… Refaire l'architecture du fichier si necessaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Heading text to the BoxInfo Page </t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,14 +207,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -445,15 +442,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -467,66 +483,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -539,12 +504,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -563,19 +522,96 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
-    <cellStyle name="60% - Accent6" xfId="4" builtinId="52"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G31"/>
+  <dimension ref="C2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +937,7 @@
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="8.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="54.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="55" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -916,287 +952,284 @@
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="14">
+      <c r="C4" s="18">
         <v>42530</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="15"/>
-      <c r="D5" s="27" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="19"/>
+      <c r="D6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="20"/>
+      <c r="D7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="21">
+        <v>42531</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="15"/>
-      <c r="D6" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
+    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="22"/>
+      <c r="D9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="22"/>
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="22"/>
+      <c r="D11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="21">
+        <v>42534</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="16"/>
-      <c r="D7" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="6" t="s">
+    <row r="13" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="22"/>
+      <c r="D13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="23"/>
+      <c r="D14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="17">
-        <v>42531</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="8" t="s">
+    <row r="16" spans="3:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="25"/>
+      <c r="D16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="25"/>
+      <c r="D17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="34" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="18"/>
-      <c r="D9" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="9" t="s">
+    <row r="18" spans="3:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="25"/>
+      <c r="D18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="34" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="18"/>
-      <c r="D10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="9" t="s">
+    <row r="19" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="26"/>
+      <c r="D19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="18"/>
-      <c r="D11" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="11" t="s">
+    <row r="20" spans="3:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C22" s="25"/>
+      <c r="D22" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="17">
-        <v>42534</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="18"/>
-      <c r="D13" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="19"/>
-      <c r="D14" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="21"/>
-      <c r="D16" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="25"/>
+      <c r="D23" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="28"/>
+    </row>
+    <row r="24" spans="3:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="25"/>
+      <c r="D24" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="42">
+        <v>0.7</v>
+      </c>
+      <c r="F24" s="29"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="25"/>
+      <c r="D25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="21"/>
-      <c r="D17" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="21"/>
-      <c r="D18" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="22"/>
-      <c r="D19" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="24" t="s">
+    <row r="26" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="25"/>
+      <c r="D26" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="38"/>
-    </row>
-    <row r="22" spans="3:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C22" s="38"/>
-      <c r="D22" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="38"/>
-    </row>
-    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="38"/>
-      <c r="D23" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="7" t="s">
+    </row>
+    <row r="27" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="25"/>
+      <c r="D27" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C28" s="25"/>
+      <c r="D28" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="25"/>
+      <c r="D29" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="38"/>
-    </row>
-    <row r="24" spans="3:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="38"/>
-      <c r="D24" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="39"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="38"/>
-      <c r="D25" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="38"/>
-      <c r="D26" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="38"/>
-      <c r="D27" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C28" s="38"/>
-      <c r="D28" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="38"/>
-      <c r="D29" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="7" t="s">
+    </row>
+    <row r="30" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="25"/>
+      <c r="D30" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C30" s="38"/>
-      <c r="D30" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="7" t="s">
+    <row r="31" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="25"/>
+      <c r="D31" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="3:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="39"/>
-      <c r="D31" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="6" t="s">
+    <row r="32" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="26"/>
+      <c r="D32" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="46" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="F20:F24"/>
-    <mergeCell ref="C21:C31"/>
+    <mergeCell ref="C21:C32"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E4:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="177" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding the research of boxes and the display of the content of the boxes at any scale, also implemented the box size in adding a box in a bigger one even if this function isn't operationnal yet, the commit is to be implemented next week
</commit_message>
<xml_diff>
--- a/Objectives.xlsx
+++ b/Objectives.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Objectif</t>
   </si>
@@ -98,9 +98,6 @@
     <t>semaine 28 au 2</t>
   </si>
   <si>
-    <t>créer une nouvelle page pour mettre du contenu dans une boite existante</t>
-  </si>
-  <si>
     <t>Mettre en place la possibilité de stocker une boite dans une autre</t>
   </si>
   <si>
@@ -141,13 +138,25 @@
   </si>
   <si>
     <t xml:space="preserve">Add Heading text to the BoxInfo Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">créer une nouvelle page pour le contenu d'une boite existante </t>
+  </si>
+  <si>
+    <t>Modifier le fichier Settings et BoxInfo pour qu'elles puissent etre claires et que l'utilisation des 2 soit fluides, qu'elles soient complementaires</t>
+  </si>
+  <si>
+    <t>EN COURS</t>
+  </si>
+  <si>
+    <t>créer une nouvelle page pour mettre du contenu dans une boite existante   IL RESTE LA SAUVEGARDE DE LA BOITE ET LA GESTION DE LA LANGUE !!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,8 +192,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +232,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -271,19 +302,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -462,14 +480,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,131 +541,141 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -926,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G32"/>
+  <dimension ref="C2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,140 +1014,140 @@
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="18">
+      <c r="C4" s="30">
         <v>42530</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="19"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="43"/>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="19"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="43"/>
     </row>
     <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="20"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="44"/>
     </row>
     <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="21">
+      <c r="C8" s="33">
         <v>42531</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="42" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="22"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="22"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="22"/>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="21">
+      <c r="C12" s="33">
         <v>42534</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="42" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="22"/>
-      <c r="D13" s="16" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="23"/>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="32"/>
+      <c r="E14" s="44"/>
     </row>
     <row r="15" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="3:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25"/>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="37"/>
+      <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="3:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="25"/>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="37"/>
+      <c r="D17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="25"/>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="37"/>
+      <c r="D18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="26"/>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="38"/>
+      <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1096,125 +1158,145 @@
       <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="40">
+      <c r="E20" s="23">
         <v>0.5</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="40"/>
+    </row>
+    <row r="22" spans="3:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="37"/>
+      <c r="D22" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C23" s="37"/>
+      <c r="D23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="40"/>
+    </row>
+    <row r="24" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="37"/>
+      <c r="D24" s="26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="38" t="s">
+      <c r="E24" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="40"/>
+    </row>
+    <row r="25" spans="3:6" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="37"/>
+      <c r="D25" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="40"/>
+    </row>
+    <row r="26" spans="3:6" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="37"/>
+      <c r="D26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="3:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C22" s="25"/>
-      <c r="D22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="25"/>
-      <c r="D23" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="44" t="s">
+      <c r="E26" s="25">
+        <v>0.7</v>
+      </c>
+      <c r="F26" s="41"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="37"/>
+      <c r="D27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="37"/>
+      <c r="D28" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="28"/>
-    </row>
-    <row r="24" spans="3:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="25"/>
-      <c r="D24" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="42">
-        <v>0.7</v>
-      </c>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="25"/>
-      <c r="D25" s="11" t="s">
+      <c r="E28" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="37"/>
+      <c r="D29" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E29" s="47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="25"/>
-      <c r="D26" s="11" t="s">
+    <row r="30" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C30" s="37"/>
+      <c r="D30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="37"/>
+      <c r="D31" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="37"/>
+      <c r="D32" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="37"/>
+      <c r="D33" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="25"/>
-      <c r="D27" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C28" s="25"/>
-      <c r="D28" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="25"/>
-      <c r="D29" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C30" s="25"/>
-      <c r="D30" s="43" t="s">
+      <c r="E33" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C31" s="25"/>
-      <c r="D31" s="43" t="s">
+    </row>
+    <row r="34" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="38"/>
+      <c r="D34" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="26"/>
-      <c r="D32" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="46" t="s">
-        <v>35</v>
+      <c r="E34" s="29" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1223,8 +1305,8 @@
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="C21:C32"/>
+    <mergeCell ref="F20:F26"/>
+    <mergeCell ref="C21:C34"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E4:E7"/>

</xml_diff>